<commit_message>
More work on FSM, 24-bit split of main ROM on MC (#2)
</commit_message>
<xml_diff>
--- a/control-signal-fsm.xlsx
+++ b/control-signal-fsm.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/85f9fbf217988a6f/College/CS 2200/cs2200-proj1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jinhai Steakhouse\OneDrive\College\CS 2200\cs2200-proj1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="FSM" sheetId="1" r:id="rId1"/>
+    <sheet name="fetch" sheetId="1" r:id="rId1"/>
+    <sheet name="add" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -21,6 +22,29 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>Bit Purpose Bit Purpose Bit Purpose Bit Purpose Bit Purpose</t>
+  </si>
+  <si>
+    <t>0 NextState[0] 5 NextState[5] 10 DrOFF 15 LdB 20 RegSelHi</t>
+  </si>
+  <si>
+    <t>1 NextState[1] 6 DrREG 11 LdPC 16 LdZ 21 ALULo</t>
+  </si>
+  <si>
+    <t>2 NextState[2] 7 DrMEM 12 LdIR 17 WrREG 22 ALUHi</t>
+  </si>
+  <si>
+    <t>3 NextState[3] 8 DrALU 13 LdMAR 18 WrMEM 23 OPTest</t>
+  </si>
+  <si>
+    <t>4 NextState[4] 9 DrPC 14 LdA 19 RegSelLo 24 chkZ</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -546,7 +570,7 @@
       <xdr:row>14</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1230273" cy="264560"/>
+    <xdr:ext cx="184731" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="19" name="TextBox 18"/>
@@ -555,7 +579,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2162175" y="2781300"/>
-          <a:ext cx="1230273" cy="264560"/>
+          <a:ext cx="184731" cy="264560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -582,18 +606,6 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>DrPC, LdA, LdMAR</a:t>
-          </a:r>
           <a:endParaRPr lang="en-US">
             <a:effectLst/>
           </a:endParaRPr>
@@ -1967,27 +1979,452 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="184731" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="67" name="TextBox 66"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4229100" y="2762250"/>
+          <a:ext cx="184731" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="896271" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="TextBox 17"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7991475" y="0"/>
+          <a:ext cx="896271" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>opcode=000</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="39" name="Straight Arrow Connector 38"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3533775" y="2457450"/>
+          <a:ext cx="342900" cy="428625"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="44450">
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="943400" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="40" name="TextBox 39"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3390900" y="2171700"/>
+          <a:ext cx="943400" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>DrMEM, LdIR</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="42" name="Straight Arrow Connector 41"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1295400" y="2457450"/>
+          <a:ext cx="342900" cy="428625"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="44450">
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1230273" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="44" name="TextBox 43"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1152525" y="2171700"/>
+          <a:ext cx="1230273" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>DrPC, LdA, LdMAR</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3549433" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="46" name="TextBox 45"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1143000" y="6200775"/>
+          <a:ext cx="3549433" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Transition</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> on: (1) Next state bits, (2) Opcode, (3) BEQ ROM</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="65" name="Oval 64"/>
+        <xdr:cNvPr id="3" name="Oval 2"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10353675" y="38100"/>
+          <a:off x="933450" y="2695575"/>
           <a:ext cx="1600200" cy="1057275"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -2029,7 +2466,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>add2</a:t>
+            <a:t>add1</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2038,152 +2475,70 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="66" name="Oval 65"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12220575" y="38100"/>
-          <a:ext cx="1600200" cy="1057275"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="00B0F0"/>
-        </a:solidFill>
-        <a:ln>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="57150" y="3200400"/>
+          <a:ext cx="847725" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="44450">
           <a:solidFill>
-            <a:srgbClr val="FFFF00"/>
+            <a:schemeClr val="tx1"/>
           </a:solidFill>
+          <a:tailEnd type="triangle"/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="2400">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>add3</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="943400" cy="264560"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="67" name="TextBox 66"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4229100" y="2762250"/>
-          <a:ext cx="943400" cy="264560"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>DrMEM, LdIR</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="896271" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="18" name="TextBox 17"/>
+        <xdr:cNvPr id="5" name="TextBox 4"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7991475" y="0"/>
+          <a:off x="114300" y="2790825"/>
           <a:ext cx="896271" cy="264560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2493,10 +2848,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="U20:U25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R6" sqref="R6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="20" spans="21:21">
+      <c r="U20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="21:21">
+      <c r="U21" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="21:21">
+      <c r="U22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="21:21">
+      <c r="U23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="21:21">
+      <c r="U24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="21:21">
+      <c r="U25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
FSM corrected, each state now has 5-bit state ID (#2)
</commit_message>
<xml_diff>
--- a/control-signal-fsm.xlsx
+++ b/control-signal-fsm.xlsx
@@ -2545,6 +2545,655 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="908903" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="55" name="TextBox 54"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1200150" y="3514725"/>
+          <a:ext cx="908903" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>State: 00000</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="908903" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="56" name="TextBox 55"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3276600" y="3524250"/>
+          <a:ext cx="908903" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>State: 00001</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="908903" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="59" name="TextBox 58"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5172075" y="3552825"/>
+          <a:ext cx="908903" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>State: 00010</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="908903" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="60" name="TextBox 59"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8924925" y="666750"/>
+          <a:ext cx="908903" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>State: 00011</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="908903" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="62" name="TextBox 61"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8924925" y="1800225"/>
+          <a:ext cx="908903" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>State: 00110</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="908903" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="65" name="TextBox 64"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8924925" y="2981325"/>
+          <a:ext cx="908903" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>State: 01001</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="908903" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="66" name="TextBox 65"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8924925" y="4171950"/>
+          <a:ext cx="908903" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>State: 01100</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="908903" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="68" name="TextBox 67"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8924925" y="5314950"/>
+          <a:ext cx="908903" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>State: 10000</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="908903" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="69" name="TextBox 68"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8915400" y="6581775"/>
+          <a:ext cx="908903" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>State: 10100</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="908903" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="70" name="TextBox 69"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8924925" y="7753350"/>
+          <a:ext cx="908903" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>State: 11010</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="908903" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="71" name="TextBox 70"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8924925" y="8877300"/>
+          <a:ext cx="908903" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>State: 11100</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3366,7 +4015,7 @@
                 </a:schemeClr>
               </a:solidFill>
             </a:rPr>
-            <a:t>NextState[00011]</a:t>
+            <a:t>NextState[00100]</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -3425,7 +4074,184 @@
                 </a:schemeClr>
               </a:solidFill>
             </a:rPr>
-            <a:t>NextState[00100]</a:t>
+            <a:t>NextState[00101]</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="908903" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="TextBox 17"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1257300" y="3295650"/>
+          <a:ext cx="908903" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>State: 00011</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="908903" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="TextBox 18"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3819525" y="3295650"/>
+          <a:ext cx="908903" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>State: 00100</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="908903" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="TextBox 19"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6362700" y="3314700"/>
+          <a:ext cx="908903" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>State: 00101</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -4253,7 +5079,7 @@
                 </a:schemeClr>
               </a:solidFill>
             </a:rPr>
-            <a:t>NextState[00101]</a:t>
+            <a:t>NextState[00111]</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -4312,7 +5138,184 @@
                 </a:schemeClr>
               </a:solidFill>
             </a:rPr>
-            <a:t>NextState[00110]</a:t>
+            <a:t>NextState[01000]</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="908903" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="TextBox 16"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1257300" y="3314700"/>
+          <a:ext cx="908903" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>State: 00110</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="908903" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="TextBox 17"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3800475" y="3314700"/>
+          <a:ext cx="908903" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>State: 00111</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="908903" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="TextBox 18"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6343650" y="3314700"/>
+          <a:ext cx="908903" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>State: 01000</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -5140,7 +6143,7 @@
                 </a:schemeClr>
               </a:solidFill>
             </a:rPr>
-            <a:t>NextState[00111]</a:t>
+            <a:t>NextState[01001]</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -5200,6 +6203,183 @@
               </a:solidFill>
             </a:rPr>
             <a:t>NextState[01000]</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="908903" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="TextBox 16"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1266825" y="3314700"/>
+          <a:ext cx="908903" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>State: 01001</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="908903" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="TextBox 17"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3829050" y="3314700"/>
+          <a:ext cx="908903" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>State: 01010</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="908903" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="TextBox 18"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6362700" y="3314700"/>
+          <a:ext cx="908903" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>State: 01011</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -6387,6 +7567,242 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="908903" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="TextBox 21"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1257300" y="3314700"/>
+          <a:ext cx="908903" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>State: 01100</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="908903" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="TextBox 22"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3810000" y="3314700"/>
+          <a:ext cx="908903" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>State: 01101</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="908903" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="TextBox 23"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6381750" y="3314700"/>
+          <a:ext cx="908903" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>State: 01110</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="908903" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="TextBox 24"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8915400" y="3314700"/>
+          <a:ext cx="908903" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>State: 01111</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7568,6 +8984,242 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="908903" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="TextBox 21"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1266825" y="3305175"/>
+          <a:ext cx="908903" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>State: 10000</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="908903" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="TextBox 22"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3810000" y="3305175"/>
+          <a:ext cx="908903" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>State: 10001</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="908903" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="TextBox 23"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6353175" y="3305175"/>
+          <a:ext cx="908903" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>State: 10010</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="908903" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="TextBox 24"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8934450" y="3305175"/>
+          <a:ext cx="908903" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>State: 10011</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -9579,6 +11231,360 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="908903" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="38" name="TextBox 37"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1247775" y="3333750"/>
+          <a:ext cx="908903" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>State: 10100</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="908903" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="39" name="TextBox 38"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3819525" y="3333750"/>
+          <a:ext cx="908903" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>State: 10101</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="908903" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="40" name="TextBox 39"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6400800" y="3333750"/>
+          <a:ext cx="908903" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>State: 10110</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="908903" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="41" name="TextBox 40"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8934450" y="2590800"/>
+          <a:ext cx="908903" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>State: 10111</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="908903" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="42" name="TextBox 41"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11487150" y="2609850"/>
+          <a:ext cx="908903" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>State: 11000</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="908903" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="43" name="TextBox 42"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14077950" y="2628900"/>
+          <a:ext cx="908903" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>State: 11001</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -10172,6 +12178,124 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="908903" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="TextBox 12"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1257300" y="3324225"/>
+          <a:ext cx="908903" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>State: 11010</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="908903" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="TextBox 13"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3800475" y="3324225"/>
+          <a:ext cx="908903" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>State: 11011</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -10586,6 +12710,65 @@
               </a:solidFill>
             </a:rPr>
             <a:t>opcode=111</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="908903" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="TextBox 8"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1276350" y="3314700"/>
+          <a:ext cx="908903" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>State: 11100</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -10861,7 +13044,7 @@
   <dimension ref="U20:U25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10907,7 +13090,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10922,7 +13105,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10937,7 +13120,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10952,7 +13135,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10967,7 +13150,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10982,7 +13165,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T28" sqref="T28"/>
+      <selection activeCell="X19" sqref="X19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10998,7 +13181,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S30" sqref="S30"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11014,7 +13197,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Edited state names to start from 0, start microcode (#2)
</commit_message>
<xml_diff>
--- a/control-signal-fsm.xlsx
+++ b/control-signal-fsm.xlsx
@@ -169,7 +169,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>fetch1</a:t>
+            <a:t>fetch0</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -238,7 +238,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>fetch2</a:t>
+            <a:t>fetch1</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -307,7 +307,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>fetch3</a:t>
+            <a:t>fetch2</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -691,7 +691,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>add1</a:t>
+            <a:t>add0</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -760,7 +760,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>addi1</a:t>
+            <a:t>addi0</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -829,7 +829,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>lw1</a:t>
+            <a:t>lw0</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -898,7 +898,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>beq1</a:t>
+            <a:t>beq0</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -967,7 +967,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>jalr1</a:t>
+            <a:t>jalr0</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1036,7 +1036,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>halt1</a:t>
+            <a:t>halt</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1700,7 +1700,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>nand1</a:t>
+            <a:t>nand0</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1769,7 +1769,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>sw1</a:t>
+            <a:t>sw0</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -3261,7 +3261,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>add1</a:t>
+            <a:t>add0</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -3439,7 +3439,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>add2</a:t>
+            <a:t>add1</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -3558,7 +3558,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>add3</a:t>
+            <a:t>add2</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -4325,7 +4325,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>nand1</a:t>
+            <a:t>nand0</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -4503,7 +4503,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>nand2</a:t>
+            <a:t>nand1</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -4622,7 +4622,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>nand3</a:t>
+            <a:t>nand2</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -5389,7 +5389,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>addi1</a:t>
+            <a:t>addi0</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -5567,7 +5567,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>addi2</a:t>
+            <a:t>addi1</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -5686,7 +5686,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>addi3</a:t>
+            <a:t>addi2</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -6453,7 +6453,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>lw1</a:t>
+            <a:t>lw0</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -6631,7 +6631,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>lw2</a:t>
+            <a:t>lw1</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -6750,7 +6750,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>lw3</a:t>
+            <a:t>lw2</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -7335,7 +7335,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>lw4</a:t>
+            <a:t>lw3</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -7870,7 +7870,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>sw1</a:t>
+            <a:t>sw0</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -8048,7 +8048,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>sw2</a:t>
+            <a:t>sw1</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -8167,7 +8167,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>sw3</a:t>
+            <a:t>sw2</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -8752,7 +8752,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>sw4</a:t>
+            <a:t>sw3</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -9287,7 +9287,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>beq1</a:t>
+            <a:t>beq0</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -9465,7 +9465,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>beq2</a:t>
+            <a:t>beq1</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -9584,7 +9584,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>beq3</a:t>
+            <a:t>beq2</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -10181,7 +10181,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>beq4</a:t>
+            <a:t>beq3</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -10584,7 +10584,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>beq5</a:t>
+            <a:t>beq4</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -10878,7 +10878,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>beq6</a:t>
+            <a:t>beq5</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -11652,7 +11652,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>jalr1</a:t>
+            <a:t>jalr0</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -11830,7 +11830,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>jalr2</a:t>
+            <a:t>jalr1</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -13043,7 +13043,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="U20:U25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Completed fetch->add microcode, corrected FSM-add (#2)
</commit_message>
<xml_diff>
--- a/control-signal-fsm.xlsx
+++ b/control-signal-fsm.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="fetch" sheetId="1" r:id="rId1"/>
@@ -3950,7 +3950,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>func=01, DrALU, WrREG, regno=00</a:t>
+            <a:t>func=00, DrALU, WrREG, regno=00</a:t>
           </a:r>
           <a:endParaRPr lang="en-US">
             <a:solidFill>
@@ -13043,7 +13043,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="U20:U25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
@@ -13089,7 +13089,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Saved changes, placeholder for more dev tomorrow (#2)
</commit_message>
<xml_diff>
--- a/control-signal-fsm.xlsx
+++ b/control-signal-fsm.xlsx
@@ -13044,7 +13044,7 @@
   <dimension ref="U20:U25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13090,7 +13090,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Complete microcode up to jalr0, corrected FSM, connect offset (#2)
</commit_message>
<xml_diff>
--- a/control-signal-fsm.xlsx
+++ b/control-signal-fsm.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="fetch" sheetId="1" r:id="rId1"/>
@@ -9814,7 +9814,7 @@
       <xdr:row>9</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1451936" cy="264560"/>
+    <xdr:ext cx="1447063" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="12" name="TextBox 11"/>
@@ -9823,7 +9823,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4000500" y="1876425"/>
-          <a:ext cx="1451936" cy="264560"/>
+          <a:ext cx="1447063" cy="264560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9860,7 +9860,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>regno=01, DrREG, LdA</a:t>
+            <a:t>regno=01, DrREG, LdB</a:t>
           </a:r>
           <a:endParaRPr lang="en-US">
             <a:solidFill>
@@ -13089,7 +13089,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
@@ -13104,7 +13104,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
@@ -13119,7 +13119,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
@@ -13134,7 +13134,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="G4" workbookViewId="0">
       <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
@@ -13149,7 +13149,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
@@ -13164,7 +13164,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="X19" sqref="X19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Microcode complete, change FSM so halt stops via loop (#2)
</commit_message>
<xml_diff>
--- a/control-signal-fsm.xlsx
+++ b/control-signal-fsm.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="fetch" sheetId="1" r:id="rId1"/>
@@ -12481,122 +12481,6 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="7" name="Straight Arrow Connector 6"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="1419225" y="2209800"/>
-          <a:ext cx="342900" cy="428625"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="44450">
-          <a:solidFill>
-            <a:srgbClr val="00B050"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="593560" cy="264560"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="TextBox 7"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1524000" y="1924050"/>
-          <a:ext cx="593560" cy="264560"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" i="1">
-              <a:solidFill>
-                <a:srgbClr val="00B050"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>OpTest</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" i="1">
-            <a:solidFill>
-              <a:srgbClr val="00B050"/>
-            </a:solidFill>
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>200025</xdr:colOff>
       <xdr:row>16</xdr:row>
@@ -12664,7 +12548,7 @@
       <xdr:row>18</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="896271" cy="264560"/>
+    <xdr:ext cx="1195455" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="17" name="TextBox 16"/>
@@ -12673,7 +12557,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4133850" y="3562350"/>
-          <a:ext cx="896271" cy="264560"/>
+          <a:ext cx="1195455" cy="264560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12703,14 +12587,18 @@
           <a:r>
             <a:rPr lang="en-US" sz="1100">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="95000"/>
-                  <a:lumOff val="5000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>opcode=111</a:t>
-          </a:r>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>NextState[11100]</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -13164,7 +13052,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="X19" sqref="X19"/>
     </sheetView>
   </sheetViews>
@@ -13196,7 +13084,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Changed all registers to rising edge (#3)
</commit_message>
<xml_diff>
--- a/control-signal-fsm.xlsx
+++ b/control-signal-fsm.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="fetch" sheetId="1" r:id="rId1"/>
@@ -11990,7 +11990,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>DrPC, regno=01, WrREG</a:t>
+            <a:t>regno=01, DrPC, WrREG</a:t>
           </a:r>
           <a:endParaRPr lang="en-US">
             <a:solidFill>
@@ -12931,7 +12931,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="U20:U25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
@@ -13022,7 +13022,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="G4" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
@@ -13068,7 +13068,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
@@ -13084,7 +13084,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>

</xml_diff>